<commit_message>
Finished the admin interface
</commit_message>
<xml_diff>
--- a/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
+++ b/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn-In-Depth\Private_Vechicle_Parking\Main_Control_ECU\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65442C74-7DB2-4E54-86D7-70484DBB07FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057E58AA-AD1E-498D-BF42-15BE9971FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Test ID</t>
   </si>
@@ -116,6 +116,19 @@
   </si>
   <si>
     <t>#'</t>
+  </si>
+  <si>
+    <t>Validate functionality of Admin Interface</t>
+  </si>
+  <si>
+    <t>Admin_Interface_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that I can login </t>
+  </si>
+  <si>
+    <t>userID = "1234"
+password = "0000"</t>
   </si>
 </sst>
 </file>
@@ -200,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -242,6 +255,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -257,35 +276,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -298,6 +312,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -358,21 +392,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -418,6 +442,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -773,286 +827,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1230,9 +1004,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1270,7 +1044,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1376,7 +1150,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1518,7 +1292,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1526,16 +1300,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="11" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
@@ -1588,106 +1362,106 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="18"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="18"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="18"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="18"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="13">
@@ -1714,17 +1488,17 @@
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -1757,35 +1531,46 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="C10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
+    <row r="10" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="18"/>
       <c r="C11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1798,9 +1583,9 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
@@ -1857,7 +1642,7 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+      <c r="A17" s="17"/>
       <c r="C17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
@@ -1869,19 +1654,19 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="C18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="C19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
@@ -1893,7 +1678,7 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="C20" s="2"/>
       <c r="E20" s="3"/>
       <c r="I20" s="2"/>
@@ -1902,7 +1687,7 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="18"/>
       <c r="C21" s="2"/>
       <c r="E21" s="3"/>
       <c r="I21" s="2"/>
@@ -1920,9 +1705,9 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -1952,7 +1737,7 @@
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
+      <c r="A25" s="17"/>
       <c r="C25" s="2"/>
       <c r="E25" s="8"/>
       <c r="I25" s="2"/>
@@ -1961,13 +1746,13 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="18"/>
       <c r="C26" s="2"/>
       <c r="E26" s="3"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1979,12 +1764,12 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+      <c r="A28" s="17"/>
       <c r="C28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="2"/>
@@ -1995,20 +1780,20 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
+      <c r="A29" s="18"/>
       <c r="C29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
+      <c r="A30" s="18"/>
       <c r="C30" s="2"/>
       <c r="E30" s="3"/>
       <c r="F30" s="2"/>
@@ -2019,7 +1804,7 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
+      <c r="A31" s="18"/>
       <c r="C31" s="2"/>
       <c r="E31" s="3"/>
       <c r="F31" s="2"/>
@@ -2030,7 +1815,7 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
+      <c r="A32" s="18"/>
       <c r="C32" s="2"/>
       <c r="E32" s="3"/>
       <c r="F32" s="2"/>
@@ -2041,7 +1826,7 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="18"/>
       <c r="C33" s="2"/>
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
@@ -2052,7 +1837,7 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="18"/>
       <c r="C34" s="2"/>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
@@ -2071,12 +1856,12 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
+      <c r="A36" s="17"/>
       <c r="C36" s="2"/>
       <c r="E36" s="3"/>
       <c r="F36" s="2"/>
@@ -2087,20 +1872,20 @@
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
+      <c r="A37" s="18"/>
       <c r="C37" s="2"/>
       <c r="E37" s="3"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="18"/>
       <c r="C38" s="2"/>
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
@@ -2110,23 +1895,8 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="L2:L6"/>
-    <mergeCell ref="A2:A8"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A28:A34"/>
     <mergeCell ref="M2:M6"/>
@@ -2138,337 +1908,261 @@
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="F2:F6"/>
     <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="L2:L6"/>
+    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B13:C13 I18:M18 B22:H22 I26:M26 I29:M29 A27:H27 I37:M37 A35:H35 E13:H13 B23:C23 I15:L15 B14:H14 B16:M16 B24:M24 A22:A24 B15:C15 A13:A17">
-    <cfRule type="cellIs" dxfId="92" priority="151" operator="equal">
+  <conditionalFormatting sqref="A28">
+    <cfRule type="cellIs" dxfId="69" priority="34" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="35" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="154" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="88" priority="83" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="84" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="85" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="84" priority="34" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="35" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="36" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="80" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="14" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="16" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 I3:I10 M3:M10 I11:M11 B9:H9 I12:L13 F10:H11 I14:M14 D3:D8 B10:E10 A12:H12 B11:G11 A9:A10">
-    <cfRule type="cellIs" dxfId="76" priority="289" operator="equal">
+  <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 D3:D8 B9:H9 A9:A10 B10:E10 F10:H11 B11:G11 A12:H12">
+    <cfRule type="cellIs" dxfId="61" priority="287" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="288" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="289" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="290" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 I3:I10 M3:M10 I11:M11 B9:H9 I12:L13 F10:H11 I14:M14 D3:D8 B10:E10 A12:H12 B11:G11 A9:A10">
-    <cfRule type="cellIs" dxfId="75" priority="287" operator="equal">
+  <conditionalFormatting sqref="B13:C13 E13:H13 A13:A17 B15:C15 B22:H22 B23:C23 A27:H27 A35:H35">
+    <cfRule type="cellIs" dxfId="57" priority="151" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="152" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="290" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="153" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="154" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C21">
-    <cfRule type="cellIs" dxfId="72" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="147" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="148" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="149" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="150" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:C26">
-    <cfRule type="cellIs" dxfId="68" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="79" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="80" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="81" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="82" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C34">
-    <cfRule type="cellIs" dxfId="64" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="30" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="31" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="32" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="33" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:C38">
-    <cfRule type="cellIs" dxfId="60" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E21">
-    <cfRule type="cellIs" dxfId="56" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="143" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="144" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="145" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="146" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="52" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="107" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="108" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="109" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="110" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="cellIs" dxfId="48" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="67" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="68" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="69" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="70" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:F15">
-    <cfRule type="cellIs" dxfId="44" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="175" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="176" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="177" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="178" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:F34">
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:F38">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F18">
-    <cfRule type="cellIs" dxfId="32" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="211" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="212" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="213" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="214" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17:H17">
-    <cfRule type="cellIs" dxfId="28" priority="139" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="140" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="141" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="142" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17:L17">
-    <cfRule type="cellIs" dxfId="24" priority="159" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="160" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="161" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="162" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19:L23">
-    <cfRule type="cellIs" dxfId="20" priority="123" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="124" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="125" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="126" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25:L25">
-    <cfRule type="cellIs" dxfId="16" priority="91" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="92" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="93" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="94" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:L28">
-    <cfRule type="cellIs" dxfId="12" priority="41" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J27:L28">
-    <cfRule type="cellIs" dxfId="11" priority="38" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="39" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="40" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30:L36">
-    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="23" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="24" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38:L40">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="214" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="0" priority="394" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="394" operator="equal">
       <formula>$I$31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:I29">
+    <cfRule type="cellIs" dxfId="8" priority="41" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:L38">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M11 I3:I13 B14:I14 M14 I15 B16:I16 M16 G17:I17 M18 I18:I23 A22:A25 B24:I24 M24 I25:I26 M26 I29 M29 I37 M37">
+    <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="84" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="85" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M11 I3:I13 B14:I14 M14 I15 B16:I16 M16 G17:I17 M18 I18:I23 A22:A25 B24:I24 M24 M26 M29 I37 M37">
+    <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
+      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the test cases for the add, remove and show list functionalites
</commit_message>
<xml_diff>
--- a/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
+++ b/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn-In-Depth\Private_Vechicle_Parking\Main_Control_ECU\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057E58AA-AD1E-498D-BF42-15BE9971FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FF1FA2-D2A6-4886-BD0F-E8B098262A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>Test ID</t>
   </si>
@@ -129,6 +129,124 @@
   <si>
     <t>userID = "1234"
 password = "0000"</t>
+  </si>
+  <si>
+    <t>Show the admin options menu</t>
+  </si>
+  <si>
+    <t>Functional Test</t>
+  </si>
+  <si>
+    <t>Admin_Interface_2</t>
+  </si>
+  <si>
+    <t>Validate that I can't login with wrong info</t>
+  </si>
+  <si>
+    <t>userID = "1234"
+password = "1111"</t>
+  </si>
+  <si>
+    <t>Go back to the login page and say wrong login info</t>
+  </si>
+  <si>
+    <t>Admin_Interface_3</t>
+  </si>
+  <si>
+    <t>Validate that I can't login when I exceed the max login attempts</t>
+  </si>
+  <si>
+    <t>Wrong info 3 times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go back to the the initial message </t>
+  </si>
+  <si>
+    <t>Vaildate functionality of the add ID operation</t>
+  </si>
+  <si>
+    <t>Admin_AddID_1</t>
+  </si>
+  <si>
+    <t>Validate that I can add a new ID</t>
+  </si>
+  <si>
+    <t>ID= "111"</t>
+  </si>
+  <si>
+    <t>ID stored in the system</t>
+  </si>
+  <si>
+    <t>Admin_AddID_2</t>
+  </si>
+  <si>
+    <t>Validate that I can't add a repeated ID</t>
+  </si>
+  <si>
+    <t>ID_1 =  "111"
+ID_2 = "111"</t>
+  </si>
+  <si>
+    <t>ID_1 stored
+ID_2 not stored and prints("ID already exist)</t>
+  </si>
+  <si>
+    <t>Admin_AddID_3</t>
+  </si>
+  <si>
+    <t>Validate that I can't add more than the maximum allowed IDs</t>
+  </si>
+  <si>
+    <t>MAX_IDs = 3
+store 4 different IDs</t>
+  </si>
+  <si>
+    <t>Store the first 3 and decline the fourth</t>
+  </si>
+  <si>
+    <t>Validate the functionality of the remove ID operation</t>
+  </si>
+  <si>
+    <t>Admin_RemoveID_1</t>
+  </si>
+  <si>
+    <t>Validate that I can remove an ID</t>
+  </si>
+  <si>
+    <t>Stored ID = "111"
+ID to be deleted = "111"</t>
+  </si>
+  <si>
+    <t>ID deleted successfully</t>
+  </si>
+  <si>
+    <t>Admin_RemoveID_2</t>
+  </si>
+  <si>
+    <t>Validate that I can’t remove an ID that doesn’t exist</t>
+  </si>
+  <si>
+    <t>Stored ID = "222"
+ID to be deleted = "111"</t>
+  </si>
+  <si>
+    <t>ID doesn't exist</t>
+  </si>
+  <si>
+    <t>Admin_RemoveID_3</t>
+  </si>
+  <si>
+    <t>Validate that I can't remove an ID when the list is empty</t>
+  </si>
+  <si>
+    <t>Stored ID: none
+ID to be deleted = "111"</t>
+  </si>
+  <si>
+    <t>List Empty</t>
+  </si>
+  <si>
+    <t>Validate the functionality of the show list operation</t>
   </si>
 </sst>
 </file>
@@ -213,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -261,6 +379,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -284,6 +405,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1300,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,99 +1492,99 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="19"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="18"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="19"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="20"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="21"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="18"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="19"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="20"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="18"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="19"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="18"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="19"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="15" t="s">
         <v>21</v>
       </c>
@@ -1488,7 +1618,7 @@
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1667,7 @@
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -1552,208 +1682,395 @@
       <c r="F10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="G10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="C11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="C13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="C17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="C18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="C19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="C20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="C21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="A22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
       <c r="C23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="2"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
+      <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="A24" s="19"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+      <c r="A25" s="19"/>
       <c r="C25" s="2"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="3"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="C26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="I26" s="5"/>
+      <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
@@ -1764,66 +2081,69 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
       <c r="C28" s="2"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="C29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="C30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="E30" s="8"/>
+      <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
       <c r="C31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
+      <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="C32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
@@ -1836,32 +2156,32 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19"/>
       <c r="C34" s="2"/>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
+      <c r="M34" s="5"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="A35" s="19"/>
+      <c r="C35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
+      <c r="A36" s="19"/>
       <c r="C36" s="2"/>
       <c r="E36" s="3"/>
       <c r="F36" s="2"/>
@@ -1872,20 +2192,18 @@
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
+      <c r="A37" s="19"/>
       <c r="C37" s="2"/>
       <c r="E37" s="3"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="5"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="5"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19"/>
       <c r="C38" s="2"/>
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
@@ -1895,14 +2213,75 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
+    <row r="39" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="C39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="C41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
+      <c r="C42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="C43" s="2"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A34"/>
+  <mergeCells count="18">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A33:A39"/>
     <mergeCell ref="M2:M6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -1915,7 +2294,7 @@
     <mergeCell ref="A2:A8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A28">
+  <conditionalFormatting sqref="A33">
     <cfRule type="cellIs" dxfId="69" priority="34" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1929,7 +2308,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A41">
     <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1943,7 +2322,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 D3:D8 B9:H9 A9:A10 B10:E10 F10:H11 B11:G11 A12:H12">
+  <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 D3:D8 B9:H9 A9:A10 B10:E10 F10:H12 B11:G12 A13:H13">
     <cfRule type="cellIs" dxfId="61" priority="287" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1957,7 +2336,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13 E13:H13 A13:A17 B15:C15 B22:H22 B23:C23 A27:H27 A35:H35">
+  <conditionalFormatting sqref="B14:C16 E14:H16 A14 B18:C20 B27:H27 B28:C28 A32:H32 A40:H40 A17:A18 A21:A22">
     <cfRule type="cellIs" dxfId="57" priority="151" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1971,7 +2350,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C21">
+  <conditionalFormatting sqref="B22:C26">
     <cfRule type="cellIs" dxfId="53" priority="147" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1985,7 +2364,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:C26">
+  <conditionalFormatting sqref="B30:C31">
     <cfRule type="cellIs" dxfId="49" priority="79" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -1999,7 +2378,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:C34">
+  <conditionalFormatting sqref="B33:C39">
     <cfRule type="cellIs" dxfId="45" priority="30" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2013,7 +2392,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:C38">
+  <conditionalFormatting sqref="B41:C43">
     <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2027,7 +2406,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E21">
+  <conditionalFormatting sqref="E22:E26">
     <cfRule type="cellIs" dxfId="37" priority="143" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2041,7 +2420,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E28">
     <cfRule type="cellIs" dxfId="33" priority="107" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2055,7 +2434,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
+  <conditionalFormatting sqref="E30:E31">
     <cfRule type="cellIs" dxfId="29" priority="67" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2069,7 +2448,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:F15">
+  <conditionalFormatting sqref="E18:F20">
     <cfRule type="cellIs" dxfId="25" priority="175" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2083,7 +2462,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F34">
+  <conditionalFormatting sqref="E33:F39">
     <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2097,7 +2476,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36:F38">
+  <conditionalFormatting sqref="E41:F43">
     <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2111,7 +2490,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F18">
+  <conditionalFormatting sqref="F22:F23">
     <cfRule type="cellIs" dxfId="13" priority="211" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2127,15 +2506,15 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="9" priority="394" operator="equal">
-      <formula>$I$31</formula>
+      <formula>$I$36</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25:I29">
+  <conditionalFormatting sqref="I30:I34">
     <cfRule type="cellIs" dxfId="8" priority="41" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:L38">
+  <conditionalFormatting sqref="J9:L43">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2149,7 +2528,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11 I3:I13 B14:I14 M14 I15 B16:I16 M16 G17:I17 M18 I18:I23 A22:A25 B24:I24 M24 I25:I26 M26 I29 M29 I37 M37">
+  <conditionalFormatting sqref="M3:M12 B17:I17 M17 B21:I21 M21 G22:I22 M23 I23:I28 A27:A30 B29:I29 M29 I30:I31 M31 I34 M34 I42 M42 I3:I16 I18:I20">
     <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2160,7 +2539,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M11 I3:I13 B14:I14 M14 I15 B16:I16 M16 G17:I17 M18 I18:I23 A22:A25 B24:I24 M24 M26 M29 I37 M37">
+  <conditionalFormatting sqref="M3:M12 B17:I17 M17 B21:I21 M21 G22:I22 M23 I23:I28 A27:A30 B29:I29 M29 M31 M34 I42 M42 I3:I16 I18:I20">
     <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added the test cases for SYSTICK and login timeout functionality
</commit_message>
<xml_diff>
--- a/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
+++ b/Main_Control_ECU/TestCases/Main_Control_ECU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn-In-Depth\Private_Vechicle_Parking\Main_Control_ECU\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F0C8D5-DF09-4F5B-8684-FBF92FEA52EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB91E52F-68A6-4C94-A03B-A67492C61F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
   <si>
     <t>Test ID</t>
   </si>
@@ -268,6 +268,99 @@
   </si>
   <si>
     <t>List empty</t>
+  </si>
+  <si>
+    <t>Validate the functionality of the timeout feature</t>
+  </si>
+  <si>
+    <t>Admin_LoginTimeout_0</t>
+  </si>
+  <si>
+    <t>Validate that I get timed out for the correct period of time after passing the maximum allowed number of login attempts</t>
+  </si>
+  <si>
+    <t>3 Invalid login attempts</t>
+  </si>
+  <si>
+    <t>Try again in 10 seconds</t>
+  </si>
+  <si>
+    <t>As expected</t>
+  </si>
+  <si>
+    <t>Validate the
+ functionality of the SYSTICK timer driver</t>
+  </si>
+  <si>
+    <t>SYSTICK_Init_0</t>
+  </si>
+  <si>
+    <t>Validate the init
+function</t>
+  </si>
+  <si>
+    <t>CLKSRC = internal CPU clock
+Interrupt = Disabled</t>
+  </si>
+  <si>
+    <t>SYSTCIK CLK as the CPU
+Interrupt is disabled</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
+  </si>
+  <si>
+    <t>SYSTICK_Init_1</t>
+  </si>
+  <si>
+    <t>1.STMCUBE_IDE
+2.Proteus Simulation
+3.SYSTICK MCAL driver</t>
+  </si>
+  <si>
+    <t>CLKSRC = internal CPU clock/8
+Interrupt = Enabled</t>
+  </si>
+  <si>
+    <t>SYSTCIK CLK CPU CLK/8
+Interrupt is enabled</t>
+  </si>
+  <si>
+    <t>SYSTICK_Delay_0</t>
+  </si>
+  <si>
+    <t>Validate the busy wait delay</t>
+  </si>
+  <si>
+    <t>Delay 2s with 8MHz freq</t>
+  </si>
+  <si>
+    <t>Halt the CPU for 2 seconds</t>
+  </si>
+  <si>
+    <t>SYSTICK_Delay_1</t>
+  </si>
+  <si>
+    <t>Validate the interval delay</t>
+  </si>
+  <si>
+    <t>Delay 2s with 8MHz freq
+with interrupt enabled</t>
+  </si>
+  <si>
+    <t>raise an interrupt after
+2 seconds</t>
+  </si>
+  <si>
+    <t>1.STMCUBE_IDE
+2.Proteus Simulation
+3.GPIO MCAL driver
+4.LCD HAL driver
+5.Keypad HAL driver
+6.SYSTICK MCAL driver</t>
   </si>
 </sst>
 </file>
@@ -322,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -354,11 +447,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,9 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -403,6 +502,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -427,27 +533,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="62">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -460,6 +571,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -470,6 +601,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -510,81 +651,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1418,16 +1489,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="9" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
@@ -1480,164 +1551,164 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="16" t="s">
+      <c r="J2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="17"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="19"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="21"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="17"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="19"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="17"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="19"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="17"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="19"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>1234567890</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>1234567890</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>1234567890</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="11" t="s">
+      <c r="J7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="J8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="12"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
@@ -1652,47 +1723,47 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="11" t="s">
+      <c r="J10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1701,32 +1772,32 @@
       <c r="E11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="11" t="s">
+      <c r="J11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1735,25 +1806,25 @@
       <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="J12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M12" s="5"/>
@@ -1767,109 +1838,109 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="11" t="s">
+      <c r="J14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="11" t="s">
+      <c r="J15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="11" t="s">
+      <c r="J16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1889,103 +1960,103 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>55</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="11" t="s">
+      <c r="J18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="11" t="s">
+      <c r="J19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="11" t="s">
+      <c r="J20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2005,10 +2076,10 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -2017,31 +2088,31 @@
       <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="15">
         <v>111222333</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="15">
         <v>111222333</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="11" t="s">
+      <c r="J22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -2050,30 +2121,30 @@
       <c r="E23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="16" t="s">
         <v>72</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="11" t="s">
+      <c r="J23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="29"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2088,183 +2159,282 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="C27" s="2"/>
-      <c r="E27" s="6"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="C28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="C30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+    <row r="25" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="M25" s="17"/>
+    </row>
+    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="17"/>
+    </row>
+    <row r="29" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="28"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I30" s="28"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="C31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="C32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+    <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="C33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
+      <c r="A34" s="18"/>
       <c r="C34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="E34" s="6"/>
+      <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
       <c r="C35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="C36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="A37" s="18"/>
+      <c r="C37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
+      <c r="A38" s="19"/>
       <c r="C38" s="2"/>
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
+      <c r="M38" s="5"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
+      <c r="A39" s="19"/>
       <c r="C39" s="2"/>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="5"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="5"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="19"/>
       <c r="C40" s="2"/>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
@@ -2274,16 +2444,100 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19"/>
+      <c r="C41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
+      <c r="C42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="C43" s="2"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="C45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="C46" s="2"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="5"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="C47" s="2"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A30:A36"/>
+  <mergeCells count="29">
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="J25:J30"/>
+    <mergeCell ref="K25:K30"/>
+    <mergeCell ref="L25:L30"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="H25:H27"/>
     <mergeCell ref="M2:M6"/>
-    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -2294,61 +2548,55 @@
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="L2:L6"/>
     <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A37:A43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A30 A21:A22 J9:L40">
-    <cfRule type="cellIs" dxfId="65" priority="34" operator="equal">
+  <conditionalFormatting sqref="A14 B14:C16 E14:H16 A17:A18 B18:C20 B32:C32 A36:H36 A44:H44 D26:D30 B24:H25 B31:H31 J31:L47 J9:L25">
+    <cfRule type="cellIs" dxfId="61" priority="151" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="152" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="153" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="154" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+  <conditionalFormatting sqref="A45">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M1 A2:B2 D2:M2 D3:D8 B9:H9 A9:A10 B10:E10 F10:H12 B11:G12 A13:H13">
-    <cfRule type="cellIs" dxfId="57" priority="287" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="287" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="288" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="289" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="289" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="290" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C16 E14:H16 A14 B18:C20 B24:H24 B25:C25 A29:H29 A37:H37 A17:A18">
-    <cfRule type="cellIs" dxfId="53" priority="151" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="152" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="153" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="290" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2366,7 +2614,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:C28">
+  <conditionalFormatting sqref="B34:C35">
     <cfRule type="cellIs" dxfId="45" priority="79" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2380,7 +2628,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C36">
+  <conditionalFormatting sqref="B37:C43">
     <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2394,7 +2642,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:C40">
+  <conditionalFormatting sqref="B45:C47">
     <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2408,63 +2656,63 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
-    <cfRule type="cellIs" dxfId="33" priority="143" operator="equal">
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="33" priority="107" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="108" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="109" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="110" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="29" priority="107" operator="equal">
+  <conditionalFormatting sqref="E34:E35">
+    <cfRule type="cellIs" dxfId="29" priority="67" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="68" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="69" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="110" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E28">
-    <cfRule type="cellIs" dxfId="25" priority="67" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="68" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="69" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="70" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:F20">
-    <cfRule type="cellIs" dxfId="21" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="175" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="176" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="177" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="178" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30:F36">
+  <conditionalFormatting sqref="E22:F23">
+    <cfRule type="cellIs" dxfId="21" priority="143" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="144" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="145" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="146" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37:F43">
     <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2478,7 +2726,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38:F40">
+  <conditionalFormatting sqref="E45:F47">
     <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2492,44 +2740,44 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
-    <cfRule type="cellIs" dxfId="9" priority="211" operator="equal">
+  <conditionalFormatting sqref="I1:I25 I31:I1048576">
+    <cfRule type="cellIs" dxfId="9" priority="403" operator="equal">
+      <formula>$I$40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34:I38 I22:I25 I31:I32 A24:A25">
+    <cfRule type="cellIs" dxfId="8" priority="41" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:A22 A37">
+    <cfRule type="cellIs" dxfId="7" priority="34" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="35" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I31 I22:I25">
-    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
+  <conditionalFormatting sqref="M3:M12 I3:I16 B17:I17 M17 I18:I20 B21:I21 M21 G22:H22 M23 B33:I33 M33 M35 M38 I46 M46 A32:A34">
+    <cfRule type="cellIs" dxfId="3" priority="86" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M12 B17:I17 M17 B21:I21 M21 M23 A24:A27 B26:I26 M26 I27:I28 M28 I31 M31 I39 M39 I3:I16 I18:I20 G22:I22 I23:I25">
-    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
+  <conditionalFormatting sqref="M3:M12 I3:I16 B17:I17 M17 I18:I20 B21:I21 M21 G22:I22 M23 B33:I33 M33 I34:I35 M35 I38 M38 I46 M46 A32:A34 I23:I25 A24:A25 I31:I32">
+    <cfRule type="cellIs" dxfId="2" priority="83" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="84" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M12 B17:I17 M17 B21:I21 M21 G22:H22 M23 A24:A27 B26:I26 M26 M28 M31 I39 M39 I3:I16 I18:I20">
-    <cfRule type="cellIs" dxfId="1" priority="86" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="0" priority="403" operator="equal">
-      <formula>$I$33</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>